<commit_message>
Updated FW ver to 1.1.0. Updated ErrorDescriptions.xlsx
</commit_message>
<xml_diff>
--- a/OpenBionics_Beetroot/Error Description.xlsx
+++ b/OpenBionics_Beetroot/Error Description.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Documents_D\GitHub\Firmware\Beetroot Software\OpenBionics_Beetroot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Documents_D\GitHub\Beetroot\OpenBionics_Beetroot\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2CF0967-4AE0-4685-9C0F-D69CB1239624}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Error List" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="76">
   <si>
     <t>Text</t>
   </si>
@@ -45,18 +46,12 @@
     <t>Error 001 - Unknown error</t>
   </si>
   <si>
-    <t>EEPROM is not detected during initialisation</t>
-  </si>
-  <si>
     <t>None</t>
   </si>
   <si>
     <t>No error. The program will run as normal</t>
   </si>
   <si>
-    <t>In this state during initialisation</t>
-  </si>
-  <si>
     <t>LED Colour</t>
   </si>
   <si>
@@ -75,9 +70,6 @@
     <t>Error 004 -  Finger pins fail to intialise</t>
   </si>
   <si>
-    <t>FingerLib fails to set finger _isActive</t>
-  </si>
-  <si>
     <t>Unknown error has occured</t>
   </si>
   <si>
@@ -117,9 +109,6 @@
     <t>Board settings - hand type</t>
   </si>
   <si>
-    <t>Too many serial characters received</t>
-  </si>
-  <si>
     <t>SerialControl.cpp</t>
   </si>
   <si>
@@ -153,15 +142,9 @@
     <t>Error 006 - Serial buffer overflow</t>
   </si>
   <si>
-    <t>Purple</t>
-  </si>
-  <si>
     <t>Board Settings -</t>
   </si>
   <si>
-    <t>Aqua</t>
-  </si>
-  <si>
     <t>Debug</t>
   </si>
   <si>
@@ -240,17 +223,44 @@
     <t>secondInterrupt()</t>
   </si>
   <si>
-    <t>Pink</t>
-  </si>
-  <si>
     <t>CPU temperature is greater than CPU_TEMP_MAX</t>
+  </si>
+  <si>
+    <t>Hand is initialising</t>
+  </si>
+  <si>
+    <t>EEPROM is not detected during initialisation (I2C issue)</t>
+  </si>
+  <si>
+    <t>Flashing (10Hz)</t>
+  </si>
+  <si>
+    <t>Finger.attach() has failed</t>
+  </si>
+  <si>
+    <t>Solid (5s)</t>
+  </si>
+  <si>
+    <t>Too many serial characters received. Some dropped</t>
+  </si>
+  <si>
+    <t>Yellow/Blue</t>
+  </si>
+  <si>
+    <t>Flashing (2Hz)</t>
+  </si>
+  <si>
+    <t>Red/Yellow</t>
+  </si>
+  <si>
+    <t>Flashing (5Hz)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -290,6 +300,22 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -351,7 +377,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -370,6 +396,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -379,12 +406,13 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="43">
+  <dxfs count="22">
     <dxf>
       <fill>
         <patternFill>
@@ -515,153 +543,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6600"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6600"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FFFF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1004,11 +885,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:L13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1019,63 +900,63 @@
     <col min="4" max="4" width="9.140625" customWidth="1"/>
     <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" customWidth="1"/>
     <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="56.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="13"/>
+      <c r="F2" s="14"/>
       <c r="G2" s="10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="K2" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="K2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="12"/>
+      <c r="L2" s="13"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H3" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>4</v>
@@ -1092,28 +973,28 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" t="s">
         <v>17</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="E4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>54</v>
-      </c>
       <c r="H4" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="K4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="L4" s="8" t="s">
         <v>7</v>
-      </c>
-      <c r="L4" s="8" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1121,63 +1002,63 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" t="s">
+        <v>54</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="L5" s="8" t="s">
         <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" t="s">
-        <v>60</v>
-      </c>
-      <c r="K5" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="L5" s="8" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
-      <c r="B6" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>65</v>
+      <c r="B6" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>59</v>
       </c>
       <c r="G6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H6" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1185,31 +1066,25 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" t="s">
         <v>15</v>
       </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" t="s">
-        <v>49</v>
-      </c>
-      <c r="E7" t="s">
-        <v>18</v>
-      </c>
       <c r="F7" t="s">
-        <v>58</v>
-      </c>
-      <c r="G7" t="s">
-        <v>44</v>
-      </c>
-      <c r="H7" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="K7" s="8" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1217,31 +1092,28 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" t="s">
         <v>49</v>
       </c>
-      <c r="E8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" t="s">
-        <v>55</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
+        <v>51</v>
+      </c>
+      <c r="K8" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="H8" t="s">
-        <v>57</v>
-      </c>
-      <c r="K8" s="8" t="s">
-        <v>48</v>
-      </c>
       <c r="L8" s="7" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1249,31 +1121,31 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" t="s">
         <v>41</v>
       </c>
-      <c r="C9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" t="s">
-        <v>47</v>
-      </c>
       <c r="E9" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F9" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G9" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H9" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="L9" s="7" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1281,25 +1153,25 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C10" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D10" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E10" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F10" t="s">
-        <v>70</v>
-      </c>
-      <c r="G10" t="s">
-        <v>71</v>
+        <v>64</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>72</v>
       </c>
       <c r="H10" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1307,35 +1179,25 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C11" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D11" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E11" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F11" t="s">
-        <v>70</v>
-      </c>
-      <c r="G11" t="s">
-        <v>71</v>
+        <v>64</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>74</v>
       </c>
       <c r="H11" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>10</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1422,7 +1284,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D13" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$K$4:$K$9</formula1>
     </dataValidation>
   </dataValidations>
@@ -1432,7 +1294,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1447,10 +1309,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>21</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>24</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>1</v>
@@ -1460,38 +1322,38 @@
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
         <v>23</v>
-      </c>
-      <c r="C2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="14"/>
+        <v>19</v>
+      </c>
+      <c r="B3" s="15"/>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="14"/>
+        <v>19</v>
+      </c>
+      <c r="B4" s="15"/>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>999</v>
       </c>
-      <c r="B5" s="14"/>
+      <c r="B5" s="15"/>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1499,7 +1361,7 @@
         <v>1000</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C6" s="6"/>
     </row>
@@ -1508,7 +1370,7 @@
         <v>1001</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C7" s="6"/>
     </row>
@@ -1517,7 +1379,7 @@
         <v>1002</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C8" s="6"/>
     </row>
@@ -1526,7 +1388,7 @@
         <v>1003</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C9" s="6"/>
     </row>
@@ -1535,7 +1397,7 @@
         <v>1004</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C10" s="6"/>
     </row>
@@ -1544,7 +1406,7 @@
         <v>1005</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C11" s="6"/>
     </row>
@@ -1553,7 +1415,7 @@
         <v>1006</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C12" s="6"/>
     </row>
@@ -1562,7 +1424,7 @@
         <v>1007</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C13" s="6"/>
     </row>
@@ -1571,7 +1433,7 @@
         <v>1008</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C14" s="6"/>
     </row>
@@ -1580,7 +1442,7 @@
         <v>1009</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C15" s="6"/>
     </row>
@@ -1589,10 +1451,10 @@
         <v>1010</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1600,10 +1462,10 @@
         <v>1011</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1611,10 +1473,10 @@
         <v>1012</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1622,10 +1484,10 @@
         <v>1013</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1633,10 +1495,10 @@
         <v>1014</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1644,10 +1506,10 @@
         <v>1015</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1655,10 +1517,10 @@
         <v>1016</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1666,10 +1528,10 @@
         <v>1017</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -1677,10 +1539,10 @@
         <v>1018</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -1688,10 +1550,10 @@
         <v>1019</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -1699,10 +1561,10 @@
         <v>1020</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1710,10 +1572,10 @@
         <v>1021</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -1721,7 +1583,7 @@
         <v>1022</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C28" s="6"/>
     </row>
@@ -1730,10 +1592,10 @@
         <v>1023</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>